<commit_message>
Use 'Virus Strain' column
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -375,7 +375,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="162">
   <si>
     <t>hai</t>
   </si>
@@ -800,9 +800,6 @@
     <t>BS_141426_WholeBlood_120314</t>
   </si>
   <si>
-    <t>B/Massachusetts/2/2012</t>
-  </si>
-  <si>
     <t>H1</t>
   </si>
   <si>
@@ -837,12 +834,6 @@
   </si>
   <si>
     <t>ES_Flu_year5HAI_141388_WholeBlood_101414_B2</t>
-  </si>
-  <si>
-    <t>Taxon Virus Strain</t>
-  </si>
-  <si>
-    <t>Taxon ID</t>
   </si>
   <si>
     <t>A/California/7/2009(H1N1)</t>
@@ -876,7 +867,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -915,13 +906,6 @@
       <charset val="204"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
       <u/>
       <sz val="10"/>
       <color theme="10"/>
@@ -936,7 +920,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -997,14 +981,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="8">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1068,60 +1046,19 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color theme="2"/>
-      </left>
-      <right style="medium">
-        <color theme="2"/>
-      </right>
-      <top style="medium">
-        <color theme="1"/>
-      </top>
-      <bottom style="medium">
-        <color theme="2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="2"/>
-      </left>
-      <right style="medium">
-        <color theme="2"/>
-      </right>
-      <top style="medium">
-        <color theme="2"/>
-      </top>
-      <bottom style="medium">
-        <color theme="2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="23"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color theme="1"/>
-      </top>
-      <bottom style="medium">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1171,19 +1108,16 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1514,7 +1448,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1522,10 +1456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE13"/>
+  <dimension ref="A1:AC13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U2" workbookViewId="0">
-      <selection activeCell="AD9" sqref="AD9"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AD1" sqref="AD1:AE1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1534,13 +1468,11 @@
     <col min="2" max="2" width="57.33203125" customWidth="1"/>
     <col min="3" max="3" width="46.5" customWidth="1"/>
     <col min="4" max="26" width="13.5" customWidth="1"/>
-    <col min="27" max="27" width="18" customWidth="1"/>
+    <col min="27" max="27" width="25.6640625" customWidth="1"/>
     <col min="28" max="29" width="13.5" customWidth="1"/>
-    <col min="30" max="30" width="26.6640625" customWidth="1"/>
-    <col min="31" max="31" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="38.25" customHeight="1">
+    <row r="1" spans="1:29" ht="38.25" customHeight="1" thickBot="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1551,12 +1483,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:31" ht="51" customHeight="1" thickBot="1">
+    <row r="2" spans="1:29" ht="51" customHeight="1" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:31" ht="63.75" customHeight="1" thickBot="1">
+    <row r="3" spans="1:29" ht="63.75" customHeight="1" thickBot="1">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -1644,17 +1576,11 @@
       <c r="AC3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AD3" s="19" t="s">
-        <v>154</v>
-      </c>
-      <c r="AE3" s="19" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="4" spans="1:31" ht="25" thickBot="1">
+    </row>
+    <row r="4" spans="1:29" ht="24">
       <c r="A4" s="1"/>
       <c r="B4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C4" t="s">
         <v>136</v>
@@ -1697,25 +1623,19 @@
       </c>
       <c r="Z4" s="1"/>
       <c r="AA4" s="1" t="s">
-        <v>94</v>
+        <v>156</v>
       </c>
       <c r="AB4">
         <v>16</v>
       </c>
       <c r="AC4" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="AD4" s="17" t="s">
-        <v>159</v>
-      </c>
-      <c r="AE4" s="17">
-        <v>1316510</v>
-      </c>
-    </row>
-    <row r="5" spans="1:31" ht="25" thickBot="1">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" ht="24">
       <c r="A5" s="1"/>
       <c r="B5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C5" t="s">
         <v>137</v>
@@ -1758,25 +1678,19 @@
       </c>
       <c r="Z5" s="1"/>
       <c r="AA5" s="1" t="s">
-        <v>94</v>
+        <v>157</v>
       </c>
       <c r="AB5">
         <v>64</v>
       </c>
       <c r="AC5" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="AD5" s="17" t="s">
-        <v>160</v>
-      </c>
-      <c r="AE5" s="18">
-        <v>1316510</v>
-      </c>
-    </row>
-    <row r="6" spans="1:31" ht="25" thickBot="1">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" ht="24">
       <c r="A6" s="1"/>
       <c r="B6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C6" t="s">
         <v>138</v>
@@ -1819,25 +1733,19 @@
       </c>
       <c r="Z6" s="1"/>
       <c r="AA6" s="1" t="s">
-        <v>94</v>
+        <v>158</v>
       </c>
       <c r="AB6">
         <v>8</v>
       </c>
       <c r="AC6" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="AD6" s="18" t="s">
-        <v>161</v>
-      </c>
-      <c r="AE6" s="18">
-        <v>1316510</v>
-      </c>
-    </row>
-    <row r="7" spans="1:31" ht="25" thickBot="1">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" ht="24">
       <c r="A7" s="1"/>
       <c r="B7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C7" t="s">
         <v>138</v>
@@ -1880,25 +1788,19 @@
       </c>
       <c r="Z7" s="1"/>
       <c r="AA7" s="1" t="s">
-        <v>94</v>
+        <v>160</v>
       </c>
       <c r="AB7">
         <v>8</v>
       </c>
       <c r="AC7" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="AD7" s="18" t="s">
-        <v>163</v>
-      </c>
-      <c r="AE7" s="18">
-        <v>1316510</v>
-      </c>
-    </row>
-    <row r="8" spans="1:31" ht="25" thickBot="1">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" ht="24">
       <c r="A8" s="1"/>
       <c r="B8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C8" t="s">
         <v>138</v>
@@ -1941,25 +1843,19 @@
       </c>
       <c r="Z8" s="1"/>
       <c r="AA8" s="1" t="s">
-        <v>94</v>
+        <v>161</v>
       </c>
       <c r="AB8">
         <v>8</v>
       </c>
       <c r="AC8" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="AD8" s="18" t="s">
-        <v>164</v>
-      </c>
-      <c r="AE8" s="18">
-        <v>1316510</v>
-      </c>
-    </row>
-    <row r="9" spans="1:31" ht="25" thickBot="1">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" ht="24">
       <c r="A9" s="1"/>
       <c r="B9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C9" t="s">
         <v>139</v>
@@ -2002,25 +1898,19 @@
       </c>
       <c r="Z9" s="1"/>
       <c r="AA9" s="1" t="s">
-        <v>94</v>
+        <v>159</v>
       </c>
       <c r="AB9">
         <v>32</v>
       </c>
       <c r="AC9" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="AD9" s="18" t="s">
-        <v>162</v>
-      </c>
-      <c r="AE9" s="18">
-        <v>1316510</v>
-      </c>
-    </row>
-    <row r="10" spans="1:31" ht="25" thickBot="1">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" ht="24">
       <c r="A10" s="1"/>
       <c r="B10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C10" t="s">
         <v>140</v>
@@ -2063,25 +1953,19 @@
       </c>
       <c r="Z10" s="1"/>
       <c r="AA10" s="1" t="s">
-        <v>94</v>
+        <v>153</v>
       </c>
       <c r="AB10">
         <v>256</v>
       </c>
       <c r="AC10" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="AD10" s="18" t="s">
-        <v>156</v>
-      </c>
-      <c r="AE10" s="18">
-        <v>1316510</v>
-      </c>
-    </row>
-    <row r="11" spans="1:31" ht="25" thickBot="1">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" ht="24">
       <c r="A11" s="1"/>
       <c r="B11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C11" t="s">
         <v>140</v>
@@ -2124,24 +2008,18 @@
       </c>
       <c r="Z11" s="1"/>
       <c r="AA11" s="1" t="s">
-        <v>97</v>
+        <v>154</v>
       </c>
       <c r="AB11">
         <v>128</v>
       </c>
       <c r="AC11" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="AD11" s="18" t="s">
-        <v>157</v>
-      </c>
-      <c r="AE11" s="18">
-        <v>1268360</v>
-      </c>
-    </row>
-    <row r="12" spans="1:31" ht="25" thickBot="1">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" ht="24">
       <c r="B12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C12" t="s">
         <v>140</v>
@@ -2170,24 +2048,18 @@
         <v>61</v>
       </c>
       <c r="AA12" s="1" t="s">
-        <v>141</v>
+        <v>155</v>
       </c>
       <c r="AB12">
         <v>64</v>
       </c>
       <c r="AC12" s="16" t="s">
-        <v>144</v>
-      </c>
-      <c r="AD12" s="18" t="s">
-        <v>158</v>
-      </c>
-      <c r="AE12" s="18">
-        <v>1321139</v>
-      </c>
-    </row>
-    <row r="13" spans="1:31" ht="25" thickBot="1">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" ht="24">
       <c r="B13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C13" t="s">
         <v>136</v>
@@ -2222,13 +2094,7 @@
         <v>8</v>
       </c>
       <c r="AC13" s="16" t="s">
-        <v>145</v>
-      </c>
-      <c r="AD13" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="AE13" s="18">
-        <v>604436</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Output highlighted Excel file
- refactor
- add Excel modification and output code
- add tests
- update sample file
- add example results file
- update README
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -375,7 +375,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="160">
   <si>
     <t>hai</t>
   </si>
@@ -851,16 +851,10 @@
     <t xml:space="preserve">   influenza a virus (a/california/7/2009(h1n1))   </t>
   </si>
   <si>
-    <t>homo sapiens</t>
-  </si>
-  <si>
     <t>Mycobacterium tuberculosis 210_4C15_16C1_48C1</t>
   </si>
   <si>
-    <t>man</t>
-  </si>
-  <si>
-    <t>Homo sapiens</t>
+    <t>xertayergavdaviweagiab</t>
   </si>
 </sst>
 </file>
@@ -1047,8 +1041,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1109,15 +1111,23 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1448,7 +1458,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1456,10 +1466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC13"/>
+  <dimension ref="A1:AC12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="AD1" sqref="AD1:AE1048576"/>
+      <selection activeCell="AA13" sqref="AA13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1690,10 +1700,10 @@
     <row r="6" spans="1:29" ht="24">
       <c r="A6" s="1"/>
       <c r="B6" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="C6" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>133</v>
@@ -1733,10 +1743,10 @@
       </c>
       <c r="Z6" s="1"/>
       <c r="AA6" s="1" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="AB6">
-        <v>8</v>
+        <v>256</v>
       </c>
       <c r="AC6" s="16" t="s">
         <v>141</v>
@@ -1745,10 +1755,10 @@
     <row r="7" spans="1:29" ht="24">
       <c r="A7" s="1"/>
       <c r="B7" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="C7" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>133</v>
@@ -1788,22 +1798,21 @@
       </c>
       <c r="Z7" s="1"/>
       <c r="AA7" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="AB7">
-        <v>8</v>
+        <v>128</v>
       </c>
       <c r="AC7" s="16" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:29" ht="24">
-      <c r="A8" s="1"/>
       <c r="B8" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="C8" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>133</v>
@@ -1815,22 +1824,9 @@
         <v>132</v>
       </c>
       <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
       <c r="K8" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="1"/>
-      <c r="S8" s="1"/>
-      <c r="T8" s="1"/>
-      <c r="U8" s="1"/>
       <c r="V8" s="15" t="s">
         <v>134</v>
       </c>
@@ -1841,24 +1837,22 @@
       <c r="Y8" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="Z8" s="1"/>
       <c r="AA8" s="1" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="AB8">
-        <v>8</v>
+        <v>64</v>
       </c>
       <c r="AC8" s="16" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:29" ht="24">
-      <c r="A9" s="1"/>
       <c r="B9" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="C9" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>133</v>
@@ -1870,22 +1864,9 @@
         <v>132</v>
       </c>
       <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
       <c r="K9" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
-      <c r="S9" s="1"/>
-      <c r="T9" s="1"/>
-      <c r="U9" s="1"/>
       <c r="V9" s="15" t="s">
         <v>134</v>
       </c>
@@ -1896,24 +1877,23 @@
       <c r="Y9" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="Z9" s="1"/>
-      <c r="AA9" s="1" t="s">
-        <v>159</v>
+      <c r="AA9" t="s">
+        <v>99</v>
       </c>
       <c r="AB9">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="AC9" s="16" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="10" spans="1:29" ht="24">
       <c r="A10" s="1"/>
       <c r="B10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>133</v>
@@ -1953,10 +1933,10 @@
       </c>
       <c r="Z10" s="1"/>
       <c r="AA10" s="1" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="AB10">
-        <v>256</v>
+        <v>32</v>
       </c>
       <c r="AC10" s="16" t="s">
         <v>141</v>
@@ -1965,10 +1945,10 @@
     <row r="11" spans="1:29" ht="24">
       <c r="A11" s="1"/>
       <c r="B11" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C11" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>133</v>
@@ -2008,21 +1988,22 @@
       </c>
       <c r="Z11" s="1"/>
       <c r="AA11" s="1" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="AB11">
-        <v>128</v>
+        <v>8</v>
       </c>
       <c r="AC11" s="16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:29" ht="24">
+      <c r="A12" s="1"/>
       <c r="B12" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C12" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>133</v>
@@ -2034,9 +2015,22 @@
         <v>132</v>
       </c>
       <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
       <c r="K12" s="14" t="s">
         <v>135</v>
       </c>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
       <c r="V12" s="15" t="s">
         <v>134</v>
       </c>
@@ -2047,77 +2041,36 @@
       <c r="Y12" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="AA12" s="1" t="s">
-        <v>155</v>
-      </c>
+      <c r="Z12" s="1"/>
+      <c r="AA12" s="1"/>
       <c r="AB12">
-        <v>64</v>
+        <v>8</v>
       </c>
       <c r="AC12" s="16" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="13" spans="1:29" ht="24">
-      <c r="B13" t="s">
-        <v>152</v>
-      </c>
-      <c r="C13" t="s">
-        <v>136</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="F13" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="G13" s="1"/>
-      <c r="K13" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="V13" s="15" t="s">
-        <v>134</v>
-      </c>
-      <c r="W13" s="1"/>
-      <c r="X13" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="Y13" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA13" t="s">
-        <v>99</v>
-      </c>
-      <c r="AB13">
-        <v>8</v>
-      </c>
-      <c r="AC13" s="16" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Study Time Collected Unit" error="Required value was not selected" promptTitle="Study Time Collected Unit" prompt="Please choose required value from the list" sqref="S4:S11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Study Time Collected Unit" error="Required value was not selected" promptTitle="Study Time Collected Unit" prompt="Please choose required value from the list" sqref="S4:S7 S10:S12">
       <formula1>"d.p.c.,Days,Hours,Minutes,Months,Not_Specified,Seconds,Weeks,Years"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Study Time T0 Event" error="Required value was not selected" promptTitle="Study Time T0 Event" prompt="Please choose required value from the list" sqref="T4:T11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Study Time T0 Event" error="Required value was not selected" promptTitle="Study Time T0 Event" prompt="Please choose required value from the list" sqref="T4:T7 T10:T12">
       <formula1>"Not_Specified,Other,Time of enrollment,Time of infection,Time of initial treatment,Time of initial vaccine administration"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Biological Sample Type" error="Required value was not selected" promptTitle="Biological Sample Type" prompt="Please choose required value from the list" sqref="N4:N11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Biological Sample Type" error="Required value was not selected" promptTitle="Biological Sample Type" prompt="Please choose required value from the list" sqref="N4:N7 N10:N12">
       <formula1>lookupsample_type_name</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Experiment Purpose" error="Required value was not selected" promptTitle="Experiment Purpose" prompt="Please choose required value from the list" sqref="X4:X13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Experiment Purpose" error="Required value was not selected" promptTitle="Experiment Purpose" prompt="Please choose required value from the list" sqref="X4:X12">
       <formula1>lookupexp_type_name</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Measurement Technique" error="Required value was not selected" promptTitle="Measurement Technique" prompt="Please choose required value from the list" sqref="Y4:Y13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Measurement Technique" error="Required value was not selected" promptTitle="Measurement Technique" prompt="Please choose required value from the list" sqref="Y4:Y12">
       <formula1>lookupexp_mea_tech_name</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Virus Strain" error="Preferred value was not selected" promptTitle="Virus Strain" prompt="Please choose preferred value from the list" sqref="AA4:AA12">
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Virus Strain" error="Preferred value was not selected" promptTitle="Virus Strain" prompt="Please choose preferred value from the list" sqref="AA4:AA8 AA10:AA12">
       <formula1>lookupvirus_strain</formula1>
     </dataValidation>
-    <dataValidation errorStyle="information" allowBlank="1" showErrorMessage="1" errorTitle="Choose from the list" error="Please choose a value from the list." promptTitle="Choose an array from the list" prompt="Please choose a value from the list." sqref="E4:E13"/>
+    <dataValidation errorStyle="information" allowBlank="1" showErrorMessage="1" errorTitle="Choose from the list" error="Please choose a value from the list." promptTitle="Choose an array from the list" prompt="Please choose a value from the list." sqref="E4:E12"/>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>